<commit_message>
Update feedback log (2025-09-27T00:40:03.602176)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>it didnt work at all</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-27 00:40:02</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-27T00:41:49.272850)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ryyy</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>testing x</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-09-27 00:41:48</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-27T00:50:48.945040)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>kj</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>kjhgf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-27 00:50:48</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-27T00:54:36.446033)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>yet another test</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-09-27 00:54:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-27T00:57:47.996202)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,28 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>steve</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>it worked a little</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-09-27 00:57:47</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T13:09:27.667848)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,28 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>kyle</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>we should update belt capstan pressure to 20psi</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-09-30 13:09:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T13:21:00.231676)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,28 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-09-30 13:20:59</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T13:25:44.061153)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,28 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>temp profile off on setup</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-09-30 13:25:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T13:25:50.884911)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,28 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>rxxx</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>greg</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>temp profile off on setup</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-09-30 13:25:50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T13:44:10.253384)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,28 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>r567</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>trudy</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>works as expected</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-09-30 13:44:09</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T19:45:23.566228)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -1,60 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.McPherson\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13656BB6-5024-4C5D-8002-F1F0BCC9405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Setup Number</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -396,61 +420,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Setup Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Operator</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Feedback</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>RA40</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Ben Suggs</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy that Cameron is here to deal with this. </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-09-30 19:45:22</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T19:45:31.807965)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RA40</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Ben Suggs</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy that Cameron is here to deal with this. </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-09-30 19:45:31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T20:25:44.866351)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>R000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Tim</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Test for tim</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-09-30 20:25:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T20:26:41.456250)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,28 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>r456</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>george</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>tiny tim must go</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-09-30 20:26:40</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T20:29:01.525918)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,28 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>r567</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>fred</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>very scary</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-09-30 20:29:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T20:30:57.680436)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,6 +565,28 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>r876</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>vicky</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>are we back to normal?</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2025-09-30 20:30:57</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T20:39:41.895546)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -587,6 +587,28 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>r345</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>rob</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>is this in eastern now?</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2025-09-30 16:39:41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-09-30T21:11:53.996249)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,28 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>r321</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>barry</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>testing the changes</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2025-09-30 17:11:53</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:34:39.305819)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -631,6 +631,28 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>r585</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tom</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Great news, turns out we not longer have high attenuation ever!</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:34:38</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:44:37.064165)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,6 +653,28 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>bruce</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">we might be close to ready </t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:44:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:47:41.089770)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,6 +675,28 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>lucky</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>im feeling</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:47:40</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:50:46.363288)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -697,6 +697,28 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>r585</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>infinite loop</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>fixed</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:50:45</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:51:14.489230)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,6 +719,28 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>r585</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>try</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>again</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:51:13</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:54:25.411482)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -741,6 +741,28 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>is this the way?</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:54:24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T18:55:11.931828)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -763,6 +763,28 @@
         </is>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>quick second test</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>2025-10-01 14:55:11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:11:16.394840)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -785,6 +785,28 @@
         </is>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>r585</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>timmy</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>water bath way too hot</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:11:15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:14:37.028334)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -807,6 +807,28 @@
         </is>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>richard</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>pss doesnt mention which weight to use</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:14:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:16:22.241092)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -829,6 +829,28 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>fred</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>4:16 fred</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:16:21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:20:34.669603)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -851,6 +851,28 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>r775</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>that feeling when you "had it" 5 tries ago</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:20:33</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:26:30.161641)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -873,6 +873,28 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>r585</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>this is with a feedback form</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:26:29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:31:31.069110)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -1,76 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29324"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron.McPherson\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13656BB6-5024-4C5D-8002-F1F0BCC9405A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Setup Number</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
-    <t>Feedback</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -85,46 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -412,61 +420,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="68.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Setup Number</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Operator</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Feedback</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" s="2"/>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Rxxx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Cameron McPherson</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Testing final v2 build</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:31:30</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update feedback log (2025-10-01T20:39:22.138745)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,28 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>app</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>cameron</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>testing app feedback</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-10-01 16:39:21</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-02T04:17:01.399731)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +499,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>App</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Sarah</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-10-02 00:17:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-13T16:01:45.356125)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,6 +521,28 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rg22</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Cam</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>High locality at line speed of 30mpm. Set to 20 dropped it down to passing levels</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2025-10-13 12:01:44</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update feedback log (2025-10-20T13:39:36.339741)
</commit_message>
<xml_diff>
--- a/feedback_log.xlsx
+++ b/feedback_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,28 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RE82</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Diana Razo</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>High ovality on this setup, decreased the water line from 100 to 85. Shrink is still passing with the change.</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2025-10-20 09:39:35</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>